<commit_message>
suppression de l'us lecture d'un message
</commit_message>
<xml_diff>
--- a/user_stories.xlsx
+++ b/user_stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Desktop\oc\projets\Projet_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA4FCA7-E455-46AA-8736-0F687A1CCA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A208DB0-6814-4A22-954E-16B76A4BB89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-5490" windowWidth="38620" windowHeight="21220" xr2:uid="{8FB0D089-BD03-4C1C-A3BC-FAF31A521F21}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Cas d'usage</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Critère(s) d'acceptation</t>
   </si>
   <si>
-    <t>Se connecter au site web</t>
-  </si>
-  <si>
     <t>Récupérer un mot de passe oublié</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Accéder à une conversation</t>
   </si>
   <si>
-    <t>Visualiser la lecture d'un message</t>
-  </si>
-  <si>
     <t>Ajouter un évènement/rendez-vous dans un calendrier</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>En tant qu'utilisateur, je veux retrouver une conversation avec un contact via l'interface de chat</t>
   </si>
   <si>
-    <t>En tant qu'utilisateur, je veux voir si un message a été lu via l'interface de chat</t>
-  </si>
-  <si>
     <t>En tant qu'utilisateur, je veux afficher mon calendrier via la page de calendrier</t>
   </si>
   <si>
@@ -135,73 +126,6 @@
   </si>
   <si>
     <t>En tant qu'utilisateur, je veux créer une tâche via la page de gestion des tâches</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Etant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis connecté et sur l'interface de chat
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur un onglet existant d'une conversation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je peux accéder à la conversation</t>
-    </r>
   </si>
   <si>
     <r>
@@ -775,74 +699,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> je suis connecté et sur l'interface de chat
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur un onglet existant d'une conversation et que j'acède à une conversation avec au moins un message envoyé
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Je peux visualiser si un message a été lu ou non</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Etant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> je suis connecté et sur la page de mon Calendrier
 </t>
     </r>
@@ -1260,6 +1116,76 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> je me déconnecte</t>
+    </r>
+  </si>
+  <si>
+    <t>Se connecter</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Etant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis connecté et sur l'interface de chat
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur un onglet existant d'une conversation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je peux accéder à la conversation, voir si un message que j'ai envoyé a été lu et voir l'heure d'envoi des messages</t>
     </r>
   </si>
 </sst>
@@ -1664,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8376B-63DD-4C7E-8F77-A51F5D13DE1F}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,175 +1620,164 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>41</v>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="11" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="12" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>42</v>
+      <c r="C12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>34</v>
+      <c r="C13" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>